<commit_message>
Progress on Verb Conjugator including first passing Unit Test.
</commit_message>
<xml_diff>
--- a/Non UI/data/Conjugation/Regular.xlsx
+++ b/Non UI/data/Conjugation/Regular.xlsx
@@ -134,9 +134,6 @@
     <t>פְּקַדְתֶּם</t>
   </si>
   <si>
-    <t>פְּקַדְתֶּנ</t>
-  </si>
-  <si>
     <t>פָּקַדְנוּ</t>
   </si>
   <si>
@@ -147,6 +144,9 @@
   </si>
   <si>
     <t>infinitive absolute</t>
+  </si>
+  <si>
+    <t>פְּקַדְתֶּן</t>
   </si>
 </sst>
 </file>
@@ -485,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:B37"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -625,7 +625,7 @@
         <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -639,7 +639,7 @@
         <v>16</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -773,7 +773,7 @@
     </row>
     <row r="21" spans="1:9" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>1</v>
@@ -971,7 +971,7 @@
     </row>
     <row r="36" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -983,7 +983,7 @@
     </row>
     <row r="37" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>

</xml_diff>